<commit_message>
fixing more wrong hyperlinks
</commit_message>
<xml_diff>
--- a/open_card_sorting/Opencard-Participant1.xlsx
+++ b/open_card_sorting/Opencard-Participant1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\almag\Coding\MLSD-in-the-LLM-Era\open_card_sorting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F7AA09-D19F-468C-A71C-C52E28BBC7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC518A3-4023-4797-9D91-838FF86CEE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2167,7 +2167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2190,13 +2190,14 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -7538,8 +7539,8 @@
   </sheetPr>
   <dimension ref="A1:F302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7558,11 +7559,11 @@
       <c r="B1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="22" t="s">
         <v>652</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -8029,7 +8030,9 @@
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="15"/>
-      <c r="F33" s="24"/>
+      <c r="F33" s="21">
+        <v>136</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
@@ -8123,7 +8126,7 @@
       <c r="A40" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="20" t="s">
         <v>128</v>
       </c>
       <c r="C40" s="10" t="s">
@@ -9480,7 +9483,7 @@
       <c r="A133" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="B133" s="18" t="s">
+      <c r="B133" s="25" t="s">
         <v>314</v>
       </c>
       <c r="C133" s="14" t="s">
@@ -12195,176 +12198,176 @@
     <hyperlink ref="B130" r:id="rId128" xr:uid="{00000000-0004-0000-0200-000080000000}"/>
     <hyperlink ref="B131" r:id="rId129" xr:uid="{00000000-0004-0000-0200-000081000000}"/>
     <hyperlink ref="B132" r:id="rId130" xr:uid="{00000000-0004-0000-0200-000082000000}"/>
-    <hyperlink ref="B133" r:id="rId131" xr:uid="{00000000-0004-0000-0200-000083000000}"/>
-    <hyperlink ref="B134" r:id="rId132" xr:uid="{00000000-0004-0000-0200-000084000000}"/>
-    <hyperlink ref="B135" r:id="rId133" xr:uid="{00000000-0004-0000-0200-000085000000}"/>
-    <hyperlink ref="B136" r:id="rId134" xr:uid="{00000000-0004-0000-0200-000086000000}"/>
-    <hyperlink ref="B137" r:id="rId135" xr:uid="{00000000-0004-0000-0200-000087000000}"/>
-    <hyperlink ref="B138" r:id="rId136" xr:uid="{00000000-0004-0000-0200-000088000000}"/>
-    <hyperlink ref="B139" r:id="rId137" xr:uid="{00000000-0004-0000-0200-000089000000}"/>
-    <hyperlink ref="B140" r:id="rId138" xr:uid="{00000000-0004-0000-0200-00008A000000}"/>
-    <hyperlink ref="B141" r:id="rId139" xr:uid="{00000000-0004-0000-0200-00008B000000}"/>
-    <hyperlink ref="B142" r:id="rId140" xr:uid="{00000000-0004-0000-0200-00008C000000}"/>
-    <hyperlink ref="B143" r:id="rId141" xr:uid="{00000000-0004-0000-0200-00008D000000}"/>
-    <hyperlink ref="B144" r:id="rId142" xr:uid="{00000000-0004-0000-0200-00008E000000}"/>
-    <hyperlink ref="B145" r:id="rId143" xr:uid="{00000000-0004-0000-0200-00008F000000}"/>
-    <hyperlink ref="B146" r:id="rId144" xr:uid="{00000000-0004-0000-0200-000090000000}"/>
-    <hyperlink ref="B147" r:id="rId145" xr:uid="{00000000-0004-0000-0200-000091000000}"/>
-    <hyperlink ref="B148" r:id="rId146" xr:uid="{00000000-0004-0000-0200-000092000000}"/>
-    <hyperlink ref="B149" r:id="rId147" xr:uid="{00000000-0004-0000-0200-000093000000}"/>
-    <hyperlink ref="B150" r:id="rId148" xr:uid="{00000000-0004-0000-0200-000094000000}"/>
-    <hyperlink ref="B151" r:id="rId149" xr:uid="{00000000-0004-0000-0200-000095000000}"/>
-    <hyperlink ref="B152" r:id="rId150" xr:uid="{00000000-0004-0000-0200-000096000000}"/>
-    <hyperlink ref="B153" r:id="rId151" xr:uid="{00000000-0004-0000-0200-000097000000}"/>
-    <hyperlink ref="B154" r:id="rId152" xr:uid="{00000000-0004-0000-0200-000098000000}"/>
-    <hyperlink ref="B155" r:id="rId153" xr:uid="{00000000-0004-0000-0200-000099000000}"/>
-    <hyperlink ref="B156" r:id="rId154" xr:uid="{00000000-0004-0000-0200-00009A000000}"/>
-    <hyperlink ref="B157" r:id="rId155" xr:uid="{00000000-0004-0000-0200-00009B000000}"/>
-    <hyperlink ref="B158" r:id="rId156" xr:uid="{00000000-0004-0000-0200-00009C000000}"/>
-    <hyperlink ref="B159" r:id="rId157" xr:uid="{00000000-0004-0000-0200-00009D000000}"/>
-    <hyperlink ref="B160" r:id="rId158" xr:uid="{00000000-0004-0000-0200-00009E000000}"/>
-    <hyperlink ref="B161" r:id="rId159" xr:uid="{00000000-0004-0000-0200-00009F000000}"/>
-    <hyperlink ref="B162" r:id="rId160" xr:uid="{00000000-0004-0000-0200-0000A0000000}"/>
-    <hyperlink ref="B163" r:id="rId161" xr:uid="{00000000-0004-0000-0200-0000A1000000}"/>
-    <hyperlink ref="B164" r:id="rId162" xr:uid="{00000000-0004-0000-0200-0000A2000000}"/>
-    <hyperlink ref="B165" r:id="rId163" xr:uid="{00000000-0004-0000-0200-0000A3000000}"/>
-    <hyperlink ref="B166" r:id="rId164" xr:uid="{00000000-0004-0000-0200-0000A4000000}"/>
-    <hyperlink ref="B167" r:id="rId165" xr:uid="{00000000-0004-0000-0200-0000A5000000}"/>
-    <hyperlink ref="B168" r:id="rId166" xr:uid="{00000000-0004-0000-0200-0000A6000000}"/>
-    <hyperlink ref="B169" r:id="rId167" xr:uid="{00000000-0004-0000-0200-0000A7000000}"/>
-    <hyperlink ref="B170" r:id="rId168" xr:uid="{00000000-0004-0000-0200-0000A8000000}"/>
-    <hyperlink ref="B171" r:id="rId169" xr:uid="{00000000-0004-0000-0200-0000A9000000}"/>
-    <hyperlink ref="B172" r:id="rId170" xr:uid="{00000000-0004-0000-0200-0000AA000000}"/>
-    <hyperlink ref="B173" r:id="rId171" xr:uid="{00000000-0004-0000-0200-0000AB000000}"/>
-    <hyperlink ref="B174" r:id="rId172" xr:uid="{00000000-0004-0000-0200-0000AC000000}"/>
-    <hyperlink ref="B175" r:id="rId173" xr:uid="{00000000-0004-0000-0200-0000AD000000}"/>
-    <hyperlink ref="B176" r:id="rId174" xr:uid="{00000000-0004-0000-0200-0000AE000000}"/>
-    <hyperlink ref="B177" r:id="rId175" xr:uid="{00000000-0004-0000-0200-0000AF000000}"/>
-    <hyperlink ref="B178" r:id="rId176" xr:uid="{00000000-0004-0000-0200-0000B0000000}"/>
-    <hyperlink ref="B179" r:id="rId177" xr:uid="{00000000-0004-0000-0200-0000B1000000}"/>
-    <hyperlink ref="B180" r:id="rId178" xr:uid="{00000000-0004-0000-0200-0000B2000000}"/>
-    <hyperlink ref="B181" r:id="rId179" xr:uid="{00000000-0004-0000-0200-0000B3000000}"/>
-    <hyperlink ref="B182" r:id="rId180" xr:uid="{00000000-0004-0000-0200-0000B4000000}"/>
-    <hyperlink ref="B183" r:id="rId181" xr:uid="{00000000-0004-0000-0200-0000B5000000}"/>
-    <hyperlink ref="B184" r:id="rId182" xr:uid="{00000000-0004-0000-0200-0000B6000000}"/>
-    <hyperlink ref="B185" r:id="rId183" xr:uid="{00000000-0004-0000-0200-0000B7000000}"/>
-    <hyperlink ref="B186" r:id="rId184" xr:uid="{00000000-0004-0000-0200-0000B8000000}"/>
-    <hyperlink ref="B187" r:id="rId185" xr:uid="{00000000-0004-0000-0200-0000B9000000}"/>
-    <hyperlink ref="B188" r:id="rId186" xr:uid="{00000000-0004-0000-0200-0000BA000000}"/>
-    <hyperlink ref="B189" r:id="rId187" xr:uid="{00000000-0004-0000-0200-0000BB000000}"/>
-    <hyperlink ref="B190" r:id="rId188" xr:uid="{00000000-0004-0000-0200-0000BC000000}"/>
-    <hyperlink ref="B191" r:id="rId189" xr:uid="{00000000-0004-0000-0200-0000BD000000}"/>
-    <hyperlink ref="B192" r:id="rId190" xr:uid="{00000000-0004-0000-0200-0000BE000000}"/>
-    <hyperlink ref="B193" r:id="rId191" xr:uid="{00000000-0004-0000-0200-0000BF000000}"/>
-    <hyperlink ref="B194" r:id="rId192" xr:uid="{00000000-0004-0000-0200-0000C0000000}"/>
-    <hyperlink ref="B195" r:id="rId193" xr:uid="{00000000-0004-0000-0200-0000C1000000}"/>
-    <hyperlink ref="B196" r:id="rId194" xr:uid="{00000000-0004-0000-0200-0000C2000000}"/>
-    <hyperlink ref="B197" r:id="rId195" xr:uid="{00000000-0004-0000-0200-0000C3000000}"/>
-    <hyperlink ref="B198" r:id="rId196" xr:uid="{00000000-0004-0000-0200-0000C4000000}"/>
-    <hyperlink ref="B199" r:id="rId197" xr:uid="{00000000-0004-0000-0200-0000C5000000}"/>
-    <hyperlink ref="B200" r:id="rId198" xr:uid="{00000000-0004-0000-0200-0000C6000000}"/>
-    <hyperlink ref="B201" r:id="rId199" xr:uid="{00000000-0004-0000-0200-0000C7000000}"/>
-    <hyperlink ref="B202" r:id="rId200" xr:uid="{00000000-0004-0000-0200-0000C8000000}"/>
-    <hyperlink ref="B203" r:id="rId201" xr:uid="{00000000-0004-0000-0200-0000C9000000}"/>
-    <hyperlink ref="B204" r:id="rId202" xr:uid="{00000000-0004-0000-0200-0000CA000000}"/>
-    <hyperlink ref="B205" r:id="rId203" xr:uid="{00000000-0004-0000-0200-0000CB000000}"/>
-    <hyperlink ref="B206" r:id="rId204" xr:uid="{00000000-0004-0000-0200-0000CC000000}"/>
-    <hyperlink ref="B207" r:id="rId205" xr:uid="{00000000-0004-0000-0200-0000CD000000}"/>
-    <hyperlink ref="B208" r:id="rId206" xr:uid="{00000000-0004-0000-0200-0000CE000000}"/>
-    <hyperlink ref="B209" r:id="rId207" xr:uid="{00000000-0004-0000-0200-0000CF000000}"/>
-    <hyperlink ref="B210" r:id="rId208" xr:uid="{00000000-0004-0000-0200-0000D0000000}"/>
-    <hyperlink ref="B211" r:id="rId209" xr:uid="{00000000-0004-0000-0200-0000D1000000}"/>
-    <hyperlink ref="B212" r:id="rId210" xr:uid="{00000000-0004-0000-0200-0000D2000000}"/>
-    <hyperlink ref="B213" r:id="rId211" xr:uid="{00000000-0004-0000-0200-0000D3000000}"/>
-    <hyperlink ref="B214" r:id="rId212" xr:uid="{00000000-0004-0000-0200-0000D4000000}"/>
-    <hyperlink ref="B215" r:id="rId213" xr:uid="{00000000-0004-0000-0200-0000D5000000}"/>
-    <hyperlink ref="B216" r:id="rId214" xr:uid="{00000000-0004-0000-0200-0000D6000000}"/>
-    <hyperlink ref="B217" r:id="rId215" xr:uid="{00000000-0004-0000-0200-0000D7000000}"/>
-    <hyperlink ref="B218" r:id="rId216" xr:uid="{00000000-0004-0000-0200-0000D8000000}"/>
-    <hyperlink ref="B219" r:id="rId217" xr:uid="{00000000-0004-0000-0200-0000D9000000}"/>
-    <hyperlink ref="B220" r:id="rId218" xr:uid="{00000000-0004-0000-0200-0000DA000000}"/>
-    <hyperlink ref="B221" r:id="rId219" xr:uid="{00000000-0004-0000-0200-0000DB000000}"/>
-    <hyperlink ref="B222" r:id="rId220" xr:uid="{00000000-0004-0000-0200-0000DC000000}"/>
-    <hyperlink ref="B223" r:id="rId221" xr:uid="{00000000-0004-0000-0200-0000DD000000}"/>
-    <hyperlink ref="B224" r:id="rId222" xr:uid="{00000000-0004-0000-0200-0000DE000000}"/>
-    <hyperlink ref="B225" r:id="rId223" xr:uid="{00000000-0004-0000-0200-0000DF000000}"/>
-    <hyperlink ref="B226" r:id="rId224" xr:uid="{00000000-0004-0000-0200-0000E0000000}"/>
-    <hyperlink ref="B227" r:id="rId225" xr:uid="{00000000-0004-0000-0200-0000E1000000}"/>
-    <hyperlink ref="B228" r:id="rId226" xr:uid="{00000000-0004-0000-0200-0000E2000000}"/>
-    <hyperlink ref="B229" r:id="rId227" xr:uid="{00000000-0004-0000-0200-0000E3000000}"/>
-    <hyperlink ref="B230" r:id="rId228" xr:uid="{00000000-0004-0000-0200-0000E4000000}"/>
-    <hyperlink ref="B231" r:id="rId229" xr:uid="{00000000-0004-0000-0200-0000E5000000}"/>
-    <hyperlink ref="B232" r:id="rId230" xr:uid="{00000000-0004-0000-0200-0000E6000000}"/>
-    <hyperlink ref="B233" r:id="rId231" xr:uid="{00000000-0004-0000-0200-0000E7000000}"/>
-    <hyperlink ref="B234" r:id="rId232" xr:uid="{00000000-0004-0000-0200-0000E8000000}"/>
-    <hyperlink ref="B235" r:id="rId233" xr:uid="{00000000-0004-0000-0200-0000E9000000}"/>
-    <hyperlink ref="B236" r:id="rId234" xr:uid="{00000000-0004-0000-0200-0000EA000000}"/>
-    <hyperlink ref="B237" r:id="rId235" xr:uid="{00000000-0004-0000-0200-0000EB000000}"/>
-    <hyperlink ref="B238" r:id="rId236" xr:uid="{00000000-0004-0000-0200-0000EC000000}"/>
-    <hyperlink ref="B239" r:id="rId237" xr:uid="{00000000-0004-0000-0200-0000ED000000}"/>
-    <hyperlink ref="B240" r:id="rId238" xr:uid="{00000000-0004-0000-0200-0000EE000000}"/>
-    <hyperlink ref="B241" r:id="rId239" xr:uid="{00000000-0004-0000-0200-0000EF000000}"/>
-    <hyperlink ref="B242" r:id="rId240" xr:uid="{00000000-0004-0000-0200-0000F0000000}"/>
-    <hyperlink ref="B243" r:id="rId241" xr:uid="{00000000-0004-0000-0200-0000F1000000}"/>
-    <hyperlink ref="B244" r:id="rId242" xr:uid="{00000000-0004-0000-0200-0000F2000000}"/>
-    <hyperlink ref="B245" r:id="rId243" xr:uid="{00000000-0004-0000-0200-0000F3000000}"/>
-    <hyperlink ref="B246" r:id="rId244" xr:uid="{00000000-0004-0000-0200-0000F4000000}"/>
-    <hyperlink ref="B247" r:id="rId245" xr:uid="{00000000-0004-0000-0200-0000F5000000}"/>
-    <hyperlink ref="B248" r:id="rId246" xr:uid="{00000000-0004-0000-0200-0000F6000000}"/>
-    <hyperlink ref="B249" r:id="rId247" xr:uid="{00000000-0004-0000-0200-0000F7000000}"/>
-    <hyperlink ref="B250" r:id="rId248" xr:uid="{00000000-0004-0000-0200-0000F8000000}"/>
-    <hyperlink ref="B251" r:id="rId249" xr:uid="{00000000-0004-0000-0200-0000F9000000}"/>
-    <hyperlink ref="B252" r:id="rId250" xr:uid="{00000000-0004-0000-0200-0000FA000000}"/>
-    <hyperlink ref="B253" r:id="rId251" xr:uid="{00000000-0004-0000-0200-0000FB000000}"/>
-    <hyperlink ref="B254" r:id="rId252" xr:uid="{00000000-0004-0000-0200-0000FC000000}"/>
-    <hyperlink ref="B255" r:id="rId253" xr:uid="{00000000-0004-0000-0200-0000FD000000}"/>
-    <hyperlink ref="B256" r:id="rId254" xr:uid="{00000000-0004-0000-0200-0000FE000000}"/>
-    <hyperlink ref="B257" r:id="rId255" xr:uid="{00000000-0004-0000-0200-0000FF000000}"/>
-    <hyperlink ref="B258" r:id="rId256" xr:uid="{00000000-0004-0000-0200-000000010000}"/>
-    <hyperlink ref="B259" r:id="rId257" xr:uid="{00000000-0004-0000-0200-000001010000}"/>
-    <hyperlink ref="B260" r:id="rId258" xr:uid="{00000000-0004-0000-0200-000002010000}"/>
-    <hyperlink ref="B261" r:id="rId259" xr:uid="{00000000-0004-0000-0200-000003010000}"/>
-    <hyperlink ref="B262" r:id="rId260" xr:uid="{00000000-0004-0000-0200-000004010000}"/>
-    <hyperlink ref="B263" r:id="rId261" xr:uid="{00000000-0004-0000-0200-000005010000}"/>
-    <hyperlink ref="B264" r:id="rId262" xr:uid="{00000000-0004-0000-0200-000006010000}"/>
-    <hyperlink ref="B265" r:id="rId263" xr:uid="{00000000-0004-0000-0200-000007010000}"/>
-    <hyperlink ref="B266" r:id="rId264" xr:uid="{00000000-0004-0000-0200-000008010000}"/>
-    <hyperlink ref="B267" r:id="rId265" xr:uid="{00000000-0004-0000-0200-000009010000}"/>
-    <hyperlink ref="B268" r:id="rId266" xr:uid="{00000000-0004-0000-0200-00000A010000}"/>
-    <hyperlink ref="B269" r:id="rId267" xr:uid="{00000000-0004-0000-0200-00000B010000}"/>
-    <hyperlink ref="B270" r:id="rId268" xr:uid="{00000000-0004-0000-0200-00000C010000}"/>
-    <hyperlink ref="B271" r:id="rId269" xr:uid="{00000000-0004-0000-0200-00000D010000}"/>
-    <hyperlink ref="B272" r:id="rId270" xr:uid="{00000000-0004-0000-0200-00000E010000}"/>
-    <hyperlink ref="B273" r:id="rId271" xr:uid="{00000000-0004-0000-0200-00000F010000}"/>
-    <hyperlink ref="B274" r:id="rId272" xr:uid="{00000000-0004-0000-0200-000010010000}"/>
-    <hyperlink ref="B275" r:id="rId273" xr:uid="{00000000-0004-0000-0200-000011010000}"/>
-    <hyperlink ref="B276" r:id="rId274" xr:uid="{00000000-0004-0000-0200-000012010000}"/>
-    <hyperlink ref="B277" r:id="rId275" xr:uid="{00000000-0004-0000-0200-000013010000}"/>
-    <hyperlink ref="B278" r:id="rId276" xr:uid="{00000000-0004-0000-0200-000014010000}"/>
-    <hyperlink ref="B279" r:id="rId277" xr:uid="{00000000-0004-0000-0200-000015010000}"/>
-    <hyperlink ref="B280" r:id="rId278" xr:uid="{00000000-0004-0000-0200-000016010000}"/>
-    <hyperlink ref="B281" r:id="rId279" xr:uid="{00000000-0004-0000-0200-000017010000}"/>
-    <hyperlink ref="B282" r:id="rId280" xr:uid="{00000000-0004-0000-0200-000018010000}"/>
-    <hyperlink ref="B283" r:id="rId281" xr:uid="{00000000-0004-0000-0200-000019010000}"/>
-    <hyperlink ref="B284" r:id="rId282" xr:uid="{00000000-0004-0000-0200-00001A010000}"/>
-    <hyperlink ref="B285" r:id="rId283" xr:uid="{00000000-0004-0000-0200-00001B010000}"/>
-    <hyperlink ref="B286" r:id="rId284" xr:uid="{00000000-0004-0000-0200-00001C010000}"/>
-    <hyperlink ref="B287" r:id="rId285" xr:uid="{00000000-0004-0000-0200-00001D010000}"/>
-    <hyperlink ref="B288" r:id="rId286" xr:uid="{00000000-0004-0000-0200-00001E010000}"/>
-    <hyperlink ref="B289" r:id="rId287" xr:uid="{00000000-0004-0000-0200-00001F010000}"/>
-    <hyperlink ref="B290" r:id="rId288" xr:uid="{00000000-0004-0000-0200-000020010000}"/>
-    <hyperlink ref="B291" r:id="rId289" xr:uid="{00000000-0004-0000-0200-000021010000}"/>
-    <hyperlink ref="B292" r:id="rId290" xr:uid="{00000000-0004-0000-0200-000022010000}"/>
-    <hyperlink ref="B293" r:id="rId291" xr:uid="{00000000-0004-0000-0200-000023010000}"/>
-    <hyperlink ref="B294" r:id="rId292" xr:uid="{00000000-0004-0000-0200-000024010000}"/>
-    <hyperlink ref="B295" r:id="rId293" xr:uid="{00000000-0004-0000-0200-000025010000}"/>
-    <hyperlink ref="B296" r:id="rId294" xr:uid="{00000000-0004-0000-0200-000026010000}"/>
-    <hyperlink ref="B297" r:id="rId295" xr:uid="{00000000-0004-0000-0200-000027010000}"/>
-    <hyperlink ref="B298" r:id="rId296" xr:uid="{00000000-0004-0000-0200-000028010000}"/>
-    <hyperlink ref="B299" r:id="rId297" xr:uid="{00000000-0004-0000-0200-000029010000}"/>
-    <hyperlink ref="B300" r:id="rId298" xr:uid="{00000000-0004-0000-0200-00002A010000}"/>
-    <hyperlink ref="B301" r:id="rId299" xr:uid="{00000000-0004-0000-0200-00002B010000}"/>
-    <hyperlink ref="B40" r:id="rId300" xr:uid="{2B044738-2866-4B62-9B11-D3EC9011B2BA}"/>
+    <hyperlink ref="B134" r:id="rId131" xr:uid="{00000000-0004-0000-0200-000084000000}"/>
+    <hyperlink ref="B135" r:id="rId132" xr:uid="{00000000-0004-0000-0200-000085000000}"/>
+    <hyperlink ref="B136" r:id="rId133" xr:uid="{00000000-0004-0000-0200-000086000000}"/>
+    <hyperlink ref="B137" r:id="rId134" xr:uid="{00000000-0004-0000-0200-000087000000}"/>
+    <hyperlink ref="B138" r:id="rId135" xr:uid="{00000000-0004-0000-0200-000088000000}"/>
+    <hyperlink ref="B139" r:id="rId136" xr:uid="{00000000-0004-0000-0200-000089000000}"/>
+    <hyperlink ref="B140" r:id="rId137" xr:uid="{00000000-0004-0000-0200-00008A000000}"/>
+    <hyperlink ref="B141" r:id="rId138" xr:uid="{00000000-0004-0000-0200-00008B000000}"/>
+    <hyperlink ref="B142" r:id="rId139" xr:uid="{00000000-0004-0000-0200-00008C000000}"/>
+    <hyperlink ref="B143" r:id="rId140" xr:uid="{00000000-0004-0000-0200-00008D000000}"/>
+    <hyperlink ref="B144" r:id="rId141" xr:uid="{00000000-0004-0000-0200-00008E000000}"/>
+    <hyperlink ref="B145" r:id="rId142" xr:uid="{00000000-0004-0000-0200-00008F000000}"/>
+    <hyperlink ref="B146" r:id="rId143" xr:uid="{00000000-0004-0000-0200-000090000000}"/>
+    <hyperlink ref="B147" r:id="rId144" xr:uid="{00000000-0004-0000-0200-000091000000}"/>
+    <hyperlink ref="B148" r:id="rId145" xr:uid="{00000000-0004-0000-0200-000092000000}"/>
+    <hyperlink ref="B149" r:id="rId146" xr:uid="{00000000-0004-0000-0200-000093000000}"/>
+    <hyperlink ref="B150" r:id="rId147" xr:uid="{00000000-0004-0000-0200-000094000000}"/>
+    <hyperlink ref="B151" r:id="rId148" xr:uid="{00000000-0004-0000-0200-000095000000}"/>
+    <hyperlink ref="B152" r:id="rId149" xr:uid="{00000000-0004-0000-0200-000096000000}"/>
+    <hyperlink ref="B153" r:id="rId150" xr:uid="{00000000-0004-0000-0200-000097000000}"/>
+    <hyperlink ref="B154" r:id="rId151" xr:uid="{00000000-0004-0000-0200-000098000000}"/>
+    <hyperlink ref="B155" r:id="rId152" xr:uid="{00000000-0004-0000-0200-000099000000}"/>
+    <hyperlink ref="B156" r:id="rId153" xr:uid="{00000000-0004-0000-0200-00009A000000}"/>
+    <hyperlink ref="B157" r:id="rId154" xr:uid="{00000000-0004-0000-0200-00009B000000}"/>
+    <hyperlink ref="B158" r:id="rId155" xr:uid="{00000000-0004-0000-0200-00009C000000}"/>
+    <hyperlink ref="B159" r:id="rId156" xr:uid="{00000000-0004-0000-0200-00009D000000}"/>
+    <hyperlink ref="B160" r:id="rId157" xr:uid="{00000000-0004-0000-0200-00009E000000}"/>
+    <hyperlink ref="B161" r:id="rId158" xr:uid="{00000000-0004-0000-0200-00009F000000}"/>
+    <hyperlink ref="B162" r:id="rId159" xr:uid="{00000000-0004-0000-0200-0000A0000000}"/>
+    <hyperlink ref="B163" r:id="rId160" xr:uid="{00000000-0004-0000-0200-0000A1000000}"/>
+    <hyperlink ref="B164" r:id="rId161" xr:uid="{00000000-0004-0000-0200-0000A2000000}"/>
+    <hyperlink ref="B165" r:id="rId162" xr:uid="{00000000-0004-0000-0200-0000A3000000}"/>
+    <hyperlink ref="B166" r:id="rId163" xr:uid="{00000000-0004-0000-0200-0000A4000000}"/>
+    <hyperlink ref="B167" r:id="rId164" xr:uid="{00000000-0004-0000-0200-0000A5000000}"/>
+    <hyperlink ref="B168" r:id="rId165" xr:uid="{00000000-0004-0000-0200-0000A6000000}"/>
+    <hyperlink ref="B169" r:id="rId166" xr:uid="{00000000-0004-0000-0200-0000A7000000}"/>
+    <hyperlink ref="B170" r:id="rId167" xr:uid="{00000000-0004-0000-0200-0000A8000000}"/>
+    <hyperlink ref="B171" r:id="rId168" xr:uid="{00000000-0004-0000-0200-0000A9000000}"/>
+    <hyperlink ref="B172" r:id="rId169" xr:uid="{00000000-0004-0000-0200-0000AA000000}"/>
+    <hyperlink ref="B173" r:id="rId170" xr:uid="{00000000-0004-0000-0200-0000AB000000}"/>
+    <hyperlink ref="B174" r:id="rId171" xr:uid="{00000000-0004-0000-0200-0000AC000000}"/>
+    <hyperlink ref="B175" r:id="rId172" xr:uid="{00000000-0004-0000-0200-0000AD000000}"/>
+    <hyperlink ref="B176" r:id="rId173" xr:uid="{00000000-0004-0000-0200-0000AE000000}"/>
+    <hyperlink ref="B177" r:id="rId174" xr:uid="{00000000-0004-0000-0200-0000AF000000}"/>
+    <hyperlink ref="B178" r:id="rId175" xr:uid="{00000000-0004-0000-0200-0000B0000000}"/>
+    <hyperlink ref="B179" r:id="rId176" xr:uid="{00000000-0004-0000-0200-0000B1000000}"/>
+    <hyperlink ref="B180" r:id="rId177" xr:uid="{00000000-0004-0000-0200-0000B2000000}"/>
+    <hyperlink ref="B181" r:id="rId178" xr:uid="{00000000-0004-0000-0200-0000B3000000}"/>
+    <hyperlink ref="B182" r:id="rId179" xr:uid="{00000000-0004-0000-0200-0000B4000000}"/>
+    <hyperlink ref="B183" r:id="rId180" xr:uid="{00000000-0004-0000-0200-0000B5000000}"/>
+    <hyperlink ref="B184" r:id="rId181" xr:uid="{00000000-0004-0000-0200-0000B6000000}"/>
+    <hyperlink ref="B185" r:id="rId182" xr:uid="{00000000-0004-0000-0200-0000B7000000}"/>
+    <hyperlink ref="B186" r:id="rId183" xr:uid="{00000000-0004-0000-0200-0000B8000000}"/>
+    <hyperlink ref="B187" r:id="rId184" xr:uid="{00000000-0004-0000-0200-0000B9000000}"/>
+    <hyperlink ref="B188" r:id="rId185" xr:uid="{00000000-0004-0000-0200-0000BA000000}"/>
+    <hyperlink ref="B189" r:id="rId186" xr:uid="{00000000-0004-0000-0200-0000BB000000}"/>
+    <hyperlink ref="B190" r:id="rId187" xr:uid="{00000000-0004-0000-0200-0000BC000000}"/>
+    <hyperlink ref="B191" r:id="rId188" xr:uid="{00000000-0004-0000-0200-0000BD000000}"/>
+    <hyperlink ref="B192" r:id="rId189" xr:uid="{00000000-0004-0000-0200-0000BE000000}"/>
+    <hyperlink ref="B193" r:id="rId190" xr:uid="{00000000-0004-0000-0200-0000BF000000}"/>
+    <hyperlink ref="B194" r:id="rId191" xr:uid="{00000000-0004-0000-0200-0000C0000000}"/>
+    <hyperlink ref="B195" r:id="rId192" xr:uid="{00000000-0004-0000-0200-0000C1000000}"/>
+    <hyperlink ref="B196" r:id="rId193" xr:uid="{00000000-0004-0000-0200-0000C2000000}"/>
+    <hyperlink ref="B197" r:id="rId194" xr:uid="{00000000-0004-0000-0200-0000C3000000}"/>
+    <hyperlink ref="B198" r:id="rId195" xr:uid="{00000000-0004-0000-0200-0000C4000000}"/>
+    <hyperlink ref="B199" r:id="rId196" xr:uid="{00000000-0004-0000-0200-0000C5000000}"/>
+    <hyperlink ref="B200" r:id="rId197" xr:uid="{00000000-0004-0000-0200-0000C6000000}"/>
+    <hyperlink ref="B201" r:id="rId198" xr:uid="{00000000-0004-0000-0200-0000C7000000}"/>
+    <hyperlink ref="B202" r:id="rId199" xr:uid="{00000000-0004-0000-0200-0000C8000000}"/>
+    <hyperlink ref="B203" r:id="rId200" xr:uid="{00000000-0004-0000-0200-0000C9000000}"/>
+    <hyperlink ref="B204" r:id="rId201" xr:uid="{00000000-0004-0000-0200-0000CA000000}"/>
+    <hyperlink ref="B205" r:id="rId202" xr:uid="{00000000-0004-0000-0200-0000CB000000}"/>
+    <hyperlink ref="B206" r:id="rId203" xr:uid="{00000000-0004-0000-0200-0000CC000000}"/>
+    <hyperlink ref="B207" r:id="rId204" xr:uid="{00000000-0004-0000-0200-0000CD000000}"/>
+    <hyperlink ref="B208" r:id="rId205" xr:uid="{00000000-0004-0000-0200-0000CE000000}"/>
+    <hyperlink ref="B209" r:id="rId206" xr:uid="{00000000-0004-0000-0200-0000CF000000}"/>
+    <hyperlink ref="B210" r:id="rId207" xr:uid="{00000000-0004-0000-0200-0000D0000000}"/>
+    <hyperlink ref="B211" r:id="rId208" xr:uid="{00000000-0004-0000-0200-0000D1000000}"/>
+    <hyperlink ref="B212" r:id="rId209" xr:uid="{00000000-0004-0000-0200-0000D2000000}"/>
+    <hyperlink ref="B213" r:id="rId210" xr:uid="{00000000-0004-0000-0200-0000D3000000}"/>
+    <hyperlink ref="B214" r:id="rId211" xr:uid="{00000000-0004-0000-0200-0000D4000000}"/>
+    <hyperlink ref="B215" r:id="rId212" xr:uid="{00000000-0004-0000-0200-0000D5000000}"/>
+    <hyperlink ref="B216" r:id="rId213" xr:uid="{00000000-0004-0000-0200-0000D6000000}"/>
+    <hyperlink ref="B217" r:id="rId214" xr:uid="{00000000-0004-0000-0200-0000D7000000}"/>
+    <hyperlink ref="B218" r:id="rId215" xr:uid="{00000000-0004-0000-0200-0000D8000000}"/>
+    <hyperlink ref="B219" r:id="rId216" xr:uid="{00000000-0004-0000-0200-0000D9000000}"/>
+    <hyperlink ref="B220" r:id="rId217" xr:uid="{00000000-0004-0000-0200-0000DA000000}"/>
+    <hyperlink ref="B221" r:id="rId218" xr:uid="{00000000-0004-0000-0200-0000DB000000}"/>
+    <hyperlink ref="B222" r:id="rId219" xr:uid="{00000000-0004-0000-0200-0000DC000000}"/>
+    <hyperlink ref="B223" r:id="rId220" xr:uid="{00000000-0004-0000-0200-0000DD000000}"/>
+    <hyperlink ref="B224" r:id="rId221" xr:uid="{00000000-0004-0000-0200-0000DE000000}"/>
+    <hyperlink ref="B225" r:id="rId222" xr:uid="{00000000-0004-0000-0200-0000DF000000}"/>
+    <hyperlink ref="B226" r:id="rId223" xr:uid="{00000000-0004-0000-0200-0000E0000000}"/>
+    <hyperlink ref="B227" r:id="rId224" xr:uid="{00000000-0004-0000-0200-0000E1000000}"/>
+    <hyperlink ref="B228" r:id="rId225" xr:uid="{00000000-0004-0000-0200-0000E2000000}"/>
+    <hyperlink ref="B229" r:id="rId226" xr:uid="{00000000-0004-0000-0200-0000E3000000}"/>
+    <hyperlink ref="B230" r:id="rId227" xr:uid="{00000000-0004-0000-0200-0000E4000000}"/>
+    <hyperlink ref="B231" r:id="rId228" xr:uid="{00000000-0004-0000-0200-0000E5000000}"/>
+    <hyperlink ref="B232" r:id="rId229" xr:uid="{00000000-0004-0000-0200-0000E6000000}"/>
+    <hyperlink ref="B233" r:id="rId230" xr:uid="{00000000-0004-0000-0200-0000E7000000}"/>
+    <hyperlink ref="B234" r:id="rId231" xr:uid="{00000000-0004-0000-0200-0000E8000000}"/>
+    <hyperlink ref="B235" r:id="rId232" xr:uid="{00000000-0004-0000-0200-0000E9000000}"/>
+    <hyperlink ref="B236" r:id="rId233" xr:uid="{00000000-0004-0000-0200-0000EA000000}"/>
+    <hyperlink ref="B237" r:id="rId234" xr:uid="{00000000-0004-0000-0200-0000EB000000}"/>
+    <hyperlink ref="B238" r:id="rId235" xr:uid="{00000000-0004-0000-0200-0000EC000000}"/>
+    <hyperlink ref="B239" r:id="rId236" xr:uid="{00000000-0004-0000-0200-0000ED000000}"/>
+    <hyperlink ref="B240" r:id="rId237" xr:uid="{00000000-0004-0000-0200-0000EE000000}"/>
+    <hyperlink ref="B241" r:id="rId238" xr:uid="{00000000-0004-0000-0200-0000EF000000}"/>
+    <hyperlink ref="B242" r:id="rId239" xr:uid="{00000000-0004-0000-0200-0000F0000000}"/>
+    <hyperlink ref="B243" r:id="rId240" xr:uid="{00000000-0004-0000-0200-0000F1000000}"/>
+    <hyperlink ref="B244" r:id="rId241" xr:uid="{00000000-0004-0000-0200-0000F2000000}"/>
+    <hyperlink ref="B245" r:id="rId242" xr:uid="{00000000-0004-0000-0200-0000F3000000}"/>
+    <hyperlink ref="B246" r:id="rId243" xr:uid="{00000000-0004-0000-0200-0000F4000000}"/>
+    <hyperlink ref="B247" r:id="rId244" xr:uid="{00000000-0004-0000-0200-0000F5000000}"/>
+    <hyperlink ref="B248" r:id="rId245" xr:uid="{00000000-0004-0000-0200-0000F6000000}"/>
+    <hyperlink ref="B249" r:id="rId246" xr:uid="{00000000-0004-0000-0200-0000F7000000}"/>
+    <hyperlink ref="B250" r:id="rId247" xr:uid="{00000000-0004-0000-0200-0000F8000000}"/>
+    <hyperlink ref="B251" r:id="rId248" xr:uid="{00000000-0004-0000-0200-0000F9000000}"/>
+    <hyperlink ref="B252" r:id="rId249" xr:uid="{00000000-0004-0000-0200-0000FA000000}"/>
+    <hyperlink ref="B253" r:id="rId250" xr:uid="{00000000-0004-0000-0200-0000FB000000}"/>
+    <hyperlink ref="B254" r:id="rId251" xr:uid="{00000000-0004-0000-0200-0000FC000000}"/>
+    <hyperlink ref="B255" r:id="rId252" xr:uid="{00000000-0004-0000-0200-0000FD000000}"/>
+    <hyperlink ref="B256" r:id="rId253" xr:uid="{00000000-0004-0000-0200-0000FE000000}"/>
+    <hyperlink ref="B257" r:id="rId254" xr:uid="{00000000-0004-0000-0200-0000FF000000}"/>
+    <hyperlink ref="B258" r:id="rId255" xr:uid="{00000000-0004-0000-0200-000000010000}"/>
+    <hyperlink ref="B259" r:id="rId256" xr:uid="{00000000-0004-0000-0200-000001010000}"/>
+    <hyperlink ref="B260" r:id="rId257" xr:uid="{00000000-0004-0000-0200-000002010000}"/>
+    <hyperlink ref="B261" r:id="rId258" xr:uid="{00000000-0004-0000-0200-000003010000}"/>
+    <hyperlink ref="B262" r:id="rId259" xr:uid="{00000000-0004-0000-0200-000004010000}"/>
+    <hyperlink ref="B263" r:id="rId260" xr:uid="{00000000-0004-0000-0200-000005010000}"/>
+    <hyperlink ref="B264" r:id="rId261" xr:uid="{00000000-0004-0000-0200-000006010000}"/>
+    <hyperlink ref="B265" r:id="rId262" xr:uid="{00000000-0004-0000-0200-000007010000}"/>
+    <hyperlink ref="B266" r:id="rId263" xr:uid="{00000000-0004-0000-0200-000008010000}"/>
+    <hyperlink ref="B267" r:id="rId264" xr:uid="{00000000-0004-0000-0200-000009010000}"/>
+    <hyperlink ref="B268" r:id="rId265" xr:uid="{00000000-0004-0000-0200-00000A010000}"/>
+    <hyperlink ref="B269" r:id="rId266" xr:uid="{00000000-0004-0000-0200-00000B010000}"/>
+    <hyperlink ref="B270" r:id="rId267" xr:uid="{00000000-0004-0000-0200-00000C010000}"/>
+    <hyperlink ref="B271" r:id="rId268" xr:uid="{00000000-0004-0000-0200-00000D010000}"/>
+    <hyperlink ref="B272" r:id="rId269" xr:uid="{00000000-0004-0000-0200-00000E010000}"/>
+    <hyperlink ref="B273" r:id="rId270" xr:uid="{00000000-0004-0000-0200-00000F010000}"/>
+    <hyperlink ref="B274" r:id="rId271" xr:uid="{00000000-0004-0000-0200-000010010000}"/>
+    <hyperlink ref="B275" r:id="rId272" xr:uid="{00000000-0004-0000-0200-000011010000}"/>
+    <hyperlink ref="B276" r:id="rId273" xr:uid="{00000000-0004-0000-0200-000012010000}"/>
+    <hyperlink ref="B277" r:id="rId274" xr:uid="{00000000-0004-0000-0200-000013010000}"/>
+    <hyperlink ref="B278" r:id="rId275" xr:uid="{00000000-0004-0000-0200-000014010000}"/>
+    <hyperlink ref="B279" r:id="rId276" xr:uid="{00000000-0004-0000-0200-000015010000}"/>
+    <hyperlink ref="B280" r:id="rId277" xr:uid="{00000000-0004-0000-0200-000016010000}"/>
+    <hyperlink ref="B281" r:id="rId278" xr:uid="{00000000-0004-0000-0200-000017010000}"/>
+    <hyperlink ref="B282" r:id="rId279" xr:uid="{00000000-0004-0000-0200-000018010000}"/>
+    <hyperlink ref="B283" r:id="rId280" xr:uid="{00000000-0004-0000-0200-000019010000}"/>
+    <hyperlink ref="B284" r:id="rId281" xr:uid="{00000000-0004-0000-0200-00001A010000}"/>
+    <hyperlink ref="B285" r:id="rId282" xr:uid="{00000000-0004-0000-0200-00001B010000}"/>
+    <hyperlink ref="B286" r:id="rId283" xr:uid="{00000000-0004-0000-0200-00001C010000}"/>
+    <hyperlink ref="B287" r:id="rId284" xr:uid="{00000000-0004-0000-0200-00001D010000}"/>
+    <hyperlink ref="B288" r:id="rId285" xr:uid="{00000000-0004-0000-0200-00001E010000}"/>
+    <hyperlink ref="B289" r:id="rId286" xr:uid="{00000000-0004-0000-0200-00001F010000}"/>
+    <hyperlink ref="B290" r:id="rId287" xr:uid="{00000000-0004-0000-0200-000020010000}"/>
+    <hyperlink ref="B291" r:id="rId288" xr:uid="{00000000-0004-0000-0200-000021010000}"/>
+    <hyperlink ref="B292" r:id="rId289" xr:uid="{00000000-0004-0000-0200-000022010000}"/>
+    <hyperlink ref="B293" r:id="rId290" xr:uid="{00000000-0004-0000-0200-000023010000}"/>
+    <hyperlink ref="B294" r:id="rId291" xr:uid="{00000000-0004-0000-0200-000024010000}"/>
+    <hyperlink ref="B295" r:id="rId292" xr:uid="{00000000-0004-0000-0200-000025010000}"/>
+    <hyperlink ref="B296" r:id="rId293" xr:uid="{00000000-0004-0000-0200-000026010000}"/>
+    <hyperlink ref="B297" r:id="rId294" xr:uid="{00000000-0004-0000-0200-000027010000}"/>
+    <hyperlink ref="B298" r:id="rId295" xr:uid="{00000000-0004-0000-0200-000028010000}"/>
+    <hyperlink ref="B299" r:id="rId296" xr:uid="{00000000-0004-0000-0200-000029010000}"/>
+    <hyperlink ref="B300" r:id="rId297" xr:uid="{00000000-0004-0000-0200-00002A010000}"/>
+    <hyperlink ref="B301" r:id="rId298" xr:uid="{00000000-0004-0000-0200-00002B010000}"/>
+    <hyperlink ref="B40" r:id="rId299" xr:uid="{2B044738-2866-4B62-9B11-D3EC9011B2BA}"/>
+    <hyperlink ref="B133" r:id="rId300" xr:uid="{00000000-0004-0000-0200-000083000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <extLst>

</xml_diff>